<commit_message>
Two modes working code
</commit_message>
<xml_diff>
--- a/backend/data/data.xlsx
+++ b/backend/data/data.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>BuildingName</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>AudioStatus</t>
+  </si>
+  <si>
+    <t>WifiStatus</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -31,6 +34,9 @@
     <t>Holden Hall</t>
   </si>
   <si>
+    <t>Inactive</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -38,9 +44,6 @@
   </si>
   <si>
     <t>Admin Building</t>
-  </si>
-  <si>
-    <t>Inactive</t>
   </si>
   <si>
     <t>Student Union Building</t>
@@ -106,7 +109,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -152,10 +155,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -466,7 +469,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -474,8 +477,9 @@
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -485,276 +489,336 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
         <v>33.5856041036936</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>-101.873726393183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4">
         <v>33.5853113913359</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>-101.872299458104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
         <v>33.5833897435391</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>-101.874906565217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
         <v>33.5815462621146</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>-101.874863649869</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
         <v>33.5815484966595</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>-101.876531983759</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
         <v>33.5822009818309</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>-101.876770700403</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
         <v>33.5819417759833</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>-101.877392972844</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4">
         <v>33.5826123814406</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>-101.87622985745</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4">
         <v>33.5806150920787</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>-101.877147483498</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4">
         <v>33.5791987035008</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>-101.877211277659</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
         <v>33.5791455552597</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>-101.876503163863</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4">
         <v>33.5805709417876</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>-101.873132424746</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4">
         <v>33.5816801515584</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>-101.872267571469</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4">
         <v>33.5829347106625</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>-101.872510337326</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
         <v>33.5813609787148</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>-101.873189323</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4">
         <v>33.5852325962025</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
         <v>-101.871325413139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="4">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4">
         <v>33.5879248668759</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>-101.87608589962</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4">
         <v>33.5857160735429</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>-101.877102481552</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4">
         <v>33.5855264749162</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>-101.875293117493</v>
       </c>
     </row>

</xml_diff>